<commit_message>
ARI deaths Released 30/10/2025
</commit_message>
<xml_diff>
--- a/Acute respiratory infection associated deaths, 2023-2025 (a)(b)(c)(d)(e).xlsx
+++ b/Acute respiratory infection associated deaths, 2023-2025 (a)(b)(c)(d)(e).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>Acute respiratory infection associated deaths, 2023-2025 (a)(b)(c)(d)(e)</t>
   </si>
@@ -100,7 +100,7 @@
     <t>a. Includes acute respiratory disease death registrations only. Numbers will differ to disease surveillance systems.</t>
   </si>
   <si>
-    <t>b. Includes all deaths (both doctor and coroner certified) that occurred and were registered by 31 August 2025.</t>
+    <t>b. Includes all deaths (both doctor and coroner certified) that occurred and were registered by 30 September 2025.</t>
   </si>
   <si>
     <t>c. All deaths involving COVID-19 in this report have been coded to ICD-10 codes U07.1-U07.2, U10.9 or U09.9. All deaths involving influenza have been coded to J09-J11. All deaths involving RSV have been coded to J12.1, J20.5, J21.0, B97.4.</t>
@@ -112,7 +112,7 @@
     <t>e. Refer to the methodology for more information regarding the data in this table.</t>
   </si>
   <si>
-    <t>Source: Australian Bureau of Statistics, Deaths due to acute respiratory infections in Australia August 2025</t>
+    <t>Source: Australian Bureau of Statistics, Deaths due to acute respiratory infections in Australia September 2025</t>
   </si>
 </sst>
 </file>
@@ -745,7 +745,7 @@
         <v>43</v>
       </c>
       <c r="F7" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G7" s="2">
         <v>122</v>
@@ -769,7 +769,7 @@
         <v>16</v>
       </c>
       <c r="N7" s="2">
-        <v>1044</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -836,16 +836,16 @@
         <v>149</v>
       </c>
       <c r="G9" s="2">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="H9" s="2">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="I9" s="2">
-        <v>100</v>
-      </c>
-      <c r="J9" t="s">
-        <v>23</v>
+        <v>195</v>
+      </c>
+      <c r="J9" s="2">
+        <v>65</v>
       </c>
       <c r="K9" t="s">
         <v>23</v>
@@ -857,7 +857,7 @@
         <v>23</v>
       </c>
       <c r="N9" s="2">
-        <v>1703</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -880,16 +880,16 @@
         <v>78</v>
       </c>
       <c r="G10" s="2">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="H10" s="2">
-        <v>309</v>
+        <v>321</v>
       </c>
       <c r="I10" s="2">
-        <v>121</v>
-      </c>
-      <c r="J10" t="s">
-        <v>23</v>
+        <v>265</v>
+      </c>
+      <c r="J10" s="2">
+        <v>105</v>
       </c>
       <c r="K10" t="s">
         <v>23</v>
@@ -901,7 +901,7 @@
         <v>23</v>
       </c>
       <c r="N10" s="2">
-        <v>898</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -918,7 +918,7 @@
         <v>22</v>
       </c>
       <c r="E11" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F11" s="2">
         <v>40</v>
@@ -927,13 +927,13 @@
         <v>64</v>
       </c>
       <c r="H11" s="2">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I11" s="2">
-        <v>38</v>
-      </c>
-      <c r="J11" t="s">
-        <v>23</v>
+        <v>89</v>
+      </c>
+      <c r="J11" s="2">
+        <v>34</v>
       </c>
       <c r="K11" t="s">
         <v>23</v>
@@ -945,7 +945,7 @@
         <v>23</v>
       </c>
       <c r="N11" s="2">
-        <v>345</v>
+        <v>433</v>
       </c>
     </row>
     <row r="13" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Reference period October 2025 Released 28/11/2025
</commit_message>
<xml_diff>
--- a/Acute respiratory infection associated deaths, 2023-2025 (a)(b)(c)(d)(e).xlsx
+++ b/Acute respiratory infection associated deaths, 2023-2025 (a)(b)(c)(d)(e).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>Acute respiratory infection associated deaths, 2023-2025 (a)(b)(c)(d)(e)</t>
   </si>
@@ -100,7 +100,7 @@
     <t>a. Includes acute respiratory disease death registrations only. Numbers will differ to disease surveillance systems.</t>
   </si>
   <si>
-    <t>b. Includes all deaths (both doctor and coroner certified) that occurred and were registered by 30 September 2025.</t>
+    <t>b. Includes all deaths (both doctor and coroner certified) that occurred and were registered by 31 October 2025.</t>
   </si>
   <si>
     <t>c. All deaths involving COVID-19 in this report have been coded to ICD-10 codes U07.1-U07.2, U10.9 or U09.9. All deaths involving influenza have been coded to J09-J11. All deaths involving RSV have been coded to J12.1, J20.5, J21.0, B97.4.</t>
@@ -112,7 +112,7 @@
     <t>e. Refer to the methodology for more information regarding the data in this table.</t>
   </si>
   <si>
-    <t>Source: Australian Bureau of Statistics, Deaths due to acute respiratory infections in Australia September 2025</t>
+    <t>Source: Australian Bureau of Statistics, Deaths due to acute respiratory infections in Australia October 2025</t>
   </si>
 </sst>
 </file>
@@ -722,10 +722,10 @@
         <v>251</v>
       </c>
       <c r="M6" s="2">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="N6" s="2">
-        <v>5103</v>
+        <v>5105</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -821,7 +821,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="2">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C9" s="2">
         <v>164</v>
@@ -836,19 +836,19 @@
         <v>149</v>
       </c>
       <c r="G9" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="H9" s="2">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="I9" s="2">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="J9" s="2">
-        <v>65</v>
-      </c>
-      <c r="K9" t="s">
-        <v>23</v>
+        <v>139</v>
+      </c>
+      <c r="K9" s="2">
+        <v>38</v>
       </c>
       <c r="L9" t="s">
         <v>23</v>
@@ -857,7 +857,7 @@
         <v>23</v>
       </c>
       <c r="N9" s="2">
-        <v>1872</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -877,22 +877,22 @@
         <v>106</v>
       </c>
       <c r="F10" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G10" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H10" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="I10" s="2">
-        <v>265</v>
+        <v>286</v>
       </c>
       <c r="J10" s="2">
-        <v>105</v>
-      </c>
-      <c r="K10" t="s">
-        <v>23</v>
+        <v>245</v>
+      </c>
+      <c r="K10" s="2">
+        <v>59</v>
       </c>
       <c r="L10" t="s">
         <v>23</v>
@@ -901,7 +901,7 @@
         <v>23</v>
       </c>
       <c r="N10" s="2">
-        <v>1162</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -924,19 +924,19 @@
         <v>40</v>
       </c>
       <c r="G11" s="2">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H11" s="2">
         <v>118</v>
       </c>
       <c r="I11" s="2">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="J11" s="2">
-        <v>34</v>
-      </c>
-      <c r="K11" t="s">
-        <v>23</v>
+        <v>77</v>
+      </c>
+      <c r="K11" s="2">
+        <v>20</v>
       </c>
       <c r="L11" t="s">
         <v>23</v>
@@ -945,7 +945,7 @@
         <v>23</v>
       </c>
       <c r="N11" s="2">
-        <v>433</v>
+        <v>506</v>
       </c>
     </row>
     <row r="13" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>